<commit_message>
commit before merging new version
</commit_message>
<xml_diff>
--- a/Standard/Assets/ConfirmList.xlsx
+++ b/Standard/Assets/ConfirmList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Share\StandardSystem\Source\Standard\Standard\Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Share\05. Standard System\Source\Standard\Standard\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1627EDC-E12C-43FA-A7BB-F87EFE4C3A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B7FC8B-AB37-4B47-8FEE-C35B70BD884C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3C0D0120-F68B-4197-AB4F-167DF88CADA8}"/>
   </bookViews>
@@ -570,6 +570,33 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -624,59 +651,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -996,8 +996,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:BK31"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection sqref="A1:H4"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AN1" sqref="AN1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5"/>
@@ -1201,51 +1201,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:63" ht="17.25" customHeight="1">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="46" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="48" t="s">
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
+      <c r="X1" s="55"/>
+      <c r="Y1" s="55"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="55"/>
+      <c r="AC1" s="55"/>
+      <c r="AD1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="AE1" s="49"/>
-      <c r="AF1" s="49"/>
-      <c r="AG1" s="49"/>
-      <c r="AH1" s="49"/>
-      <c r="AI1" s="49"/>
-      <c r="AJ1" s="49"/>
-      <c r="AK1" s="49"/>
-      <c r="AL1" s="49"/>
-      <c r="AM1" s="50"/>
+      <c r="AE1" s="58"/>
+      <c r="AF1" s="58"/>
+      <c r="AG1" s="58"/>
+      <c r="AH1" s="58"/>
+      <c r="AI1" s="58"/>
+      <c r="AJ1" s="58"/>
+      <c r="AK1" s="58"/>
+      <c r="AL1" s="58"/>
+      <c r="AM1" s="59"/>
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
@@ -1272,35 +1272,35 @@
       <c r="BK1" s="1"/>
     </row>
     <row r="2" spans="1:63" ht="17.25" customHeight="1">
-      <c r="A2" s="44"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="47"/>
-      <c r="T2" s="47"/>
-      <c r="U2" s="47"/>
-      <c r="V2" s="47"/>
-      <c r="W2" s="47"/>
-      <c r="X2" s="47"/>
-      <c r="Y2" s="47"/>
-      <c r="Z2" s="47"/>
-      <c r="AA2" s="47"/>
-      <c r="AB2" s="47"/>
-      <c r="AC2" s="47"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
+      <c r="Q2" s="56"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="56"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="56"/>
+      <c r="V2" s="56"/>
+      <c r="W2" s="56"/>
+      <c r="X2" s="56"/>
+      <c r="Y2" s="56"/>
+      <c r="Z2" s="56"/>
+      <c r="AA2" s="56"/>
+      <c r="AB2" s="56"/>
+      <c r="AC2" s="56"/>
       <c r="AD2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1341,37 +1341,37 @@
       <c r="BK2" s="1"/>
     </row>
     <row r="3" spans="1:63" ht="17.25" customHeight="1">
-      <c r="A3" s="44"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="51" t="s">
+      <c r="A3" s="53"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="51"/>
-      <c r="S3" s="51"/>
-      <c r="T3" s="51"/>
-      <c r="U3" s="51"/>
-      <c r="V3" s="51"/>
-      <c r="W3" s="51"/>
-      <c r="X3" s="51"/>
-      <c r="Y3" s="51"/>
-      <c r="Z3" s="51"/>
-      <c r="AA3" s="51"/>
-      <c r="AB3" s="51"/>
-      <c r="AC3" s="51"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60"/>
+      <c r="R3" s="60"/>
+      <c r="S3" s="60"/>
+      <c r="T3" s="60"/>
+      <c r="U3" s="60"/>
+      <c r="V3" s="60"/>
+      <c r="W3" s="60"/>
+      <c r="X3" s="60"/>
+      <c r="Y3" s="60"/>
+      <c r="Z3" s="60"/>
+      <c r="AA3" s="60"/>
+      <c r="AB3" s="60"/>
+      <c r="AC3" s="60"/>
       <c r="AD3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1412,35 +1412,35 @@
       <c r="BK3" s="1"/>
     </row>
     <row r="4" spans="1:63" ht="17.25" customHeight="1">
-      <c r="A4" s="44"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="51"/>
-      <c r="P4" s="51"/>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="51"/>
-      <c r="S4" s="51"/>
-      <c r="T4" s="51"/>
-      <c r="U4" s="51"/>
-      <c r="V4" s="51"/>
-      <c r="W4" s="51"/>
-      <c r="X4" s="51"/>
-      <c r="Y4" s="51"/>
-      <c r="Z4" s="51"/>
-      <c r="AA4" s="51"/>
-      <c r="AB4" s="51"/>
-      <c r="AC4" s="51"/>
+      <c r="A4" s="53"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
+      <c r="P4" s="60"/>
+      <c r="Q4" s="60"/>
+      <c r="R4" s="60"/>
+      <c r="S4" s="60"/>
+      <c r="T4" s="60"/>
+      <c r="U4" s="60"/>
+      <c r="V4" s="60"/>
+      <c r="W4" s="60"/>
+      <c r="X4" s="60"/>
+      <c r="Y4" s="60"/>
+      <c r="Z4" s="60"/>
+      <c r="AA4" s="60"/>
+      <c r="AB4" s="60"/>
+      <c r="AC4" s="60"/>
       <c r="AD4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1552,31 +1552,31 @@
     <row r="6" spans="1:63" ht="18" customHeight="1">
       <c r="A6" s="13"/>
       <c r="B6" s="14"/>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="54"/>
-      <c r="P6" s="54"/>
-      <c r="Q6" s="54"/>
-      <c r="R6" s="54"/>
-      <c r="S6" s="54"/>
-      <c r="T6" s="54"/>
-      <c r="U6" s="54"/>
-      <c r="V6" s="54"/>
-      <c r="W6" s="54"/>
-      <c r="X6" s="54"/>
-      <c r="Y6" s="54"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="63"/>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="63"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
+      <c r="U6" s="63"/>
+      <c r="V6" s="63"/>
+      <c r="W6" s="63"/>
+      <c r="X6" s="63"/>
+      <c r="Y6" s="63"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
       <c r="AB6" s="1" t="s">
@@ -1621,49 +1621,49 @@
     <row r="7" spans="1:63" ht="15.75" customHeight="1">
       <c r="A7" s="8"/>
       <c r="B7" s="15"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
-      <c r="M7" s="54"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="54"/>
-      <c r="P7" s="54"/>
-      <c r="Q7" s="54"/>
-      <c r="R7" s="54"/>
-      <c r="S7" s="54"/>
-      <c r="T7" s="54"/>
-      <c r="U7" s="54"/>
-      <c r="V7" s="54"/>
-      <c r="W7" s="54"/>
-      <c r="X7" s="54"/>
-      <c r="Y7" s="54"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="63"/>
+      <c r="N7" s="63"/>
+      <c r="O7" s="63"/>
+      <c r="P7" s="63"/>
+      <c r="Q7" s="63"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="63"/>
+      <c r="U7" s="63"/>
+      <c r="V7" s="63"/>
+      <c r="W7" s="63"/>
+      <c r="X7" s="63"/>
+      <c r="Y7" s="63"/>
       <c r="Z7" s="16"/>
       <c r="AA7" s="16"/>
-      <c r="AB7" s="52" t="s">
+      <c r="AB7" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="AC7" s="52"/>
-      <c r="AD7" s="52"/>
-      <c r="AE7" s="52"/>
-      <c r="AF7" s="52" t="s">
+      <c r="AC7" s="61"/>
+      <c r="AD7" s="61"/>
+      <c r="AE7" s="61"/>
+      <c r="AF7" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="AG7" s="52"/>
-      <c r="AH7" s="52"/>
-      <c r="AI7" s="52"/>
-      <c r="AJ7" s="52" t="s">
+      <c r="AG7" s="61"/>
+      <c r="AH7" s="61"/>
+      <c r="AI7" s="61"/>
+      <c r="AJ7" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="AK7" s="52"/>
-      <c r="AL7" s="52"/>
-      <c r="AM7" s="53"/>
+      <c r="AK7" s="61"/>
+      <c r="AL7" s="61"/>
+      <c r="AM7" s="62"/>
       <c r="AN7" s="1"/>
       <c r="AO7" s="1"/>
       <c r="AP7" s="1"/>
@@ -1692,42 +1692,42 @@
     <row r="8" spans="1:63" ht="15.75" customHeight="1">
       <c r="A8" s="13"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="54"/>
-      <c r="L8" s="54"/>
-      <c r="M8" s="54"/>
-      <c r="N8" s="54"/>
-      <c r="O8" s="54"/>
-      <c r="P8" s="54"/>
-      <c r="Q8" s="54"/>
-      <c r="R8" s="54"/>
-      <c r="S8" s="54"/>
-      <c r="T8" s="54"/>
-      <c r="U8" s="54"/>
-      <c r="V8" s="54"/>
-      <c r="W8" s="54"/>
-      <c r="X8" s="54"/>
-      <c r="Y8" s="54"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="63"/>
+      <c r="N8" s="63"/>
+      <c r="O8" s="63"/>
+      <c r="P8" s="63"/>
+      <c r="Q8" s="63"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="63"/>
+      <c r="U8" s="63"/>
+      <c r="V8" s="63"/>
+      <c r="W8" s="63"/>
+      <c r="X8" s="63"/>
+      <c r="Y8" s="63"/>
       <c r="AA8" s="11"/>
-      <c r="AB8" s="37"/>
-      <c r="AC8" s="37"/>
-      <c r="AD8" s="37"/>
-      <c r="AE8" s="37"/>
-      <c r="AF8" s="37"/>
-      <c r="AG8" s="37"/>
-      <c r="AH8" s="37"/>
-      <c r="AI8" s="37"/>
-      <c r="AJ8" s="37"/>
-      <c r="AK8" s="37"/>
-      <c r="AL8" s="37"/>
-      <c r="AM8" s="38"/>
+      <c r="AB8" s="46"/>
+      <c r="AC8" s="46"/>
+      <c r="AD8" s="46"/>
+      <c r="AE8" s="46"/>
+      <c r="AF8" s="46"/>
+      <c r="AG8" s="46"/>
+      <c r="AH8" s="46"/>
+      <c r="AI8" s="46"/>
+      <c r="AJ8" s="46"/>
+      <c r="AK8" s="46"/>
+      <c r="AL8" s="46"/>
+      <c r="AM8" s="47"/>
       <c r="AN8" s="1"/>
       <c r="AO8" s="1"/>
       <c r="AP8" s="1"/>
@@ -1756,43 +1756,43 @@
     <row r="9" spans="1:63" s="20" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="14"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
-      <c r="M9" s="54"/>
-      <c r="N9" s="54"/>
-      <c r="O9" s="54"/>
-      <c r="P9" s="54"/>
-      <c r="Q9" s="54"/>
-      <c r="R9" s="54"/>
-      <c r="S9" s="54"/>
-      <c r="T9" s="54"/>
-      <c r="U9" s="54"/>
-      <c r="V9" s="54"/>
-      <c r="W9" s="54"/>
-      <c r="X9" s="54"/>
-      <c r="Y9" s="54"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="63"/>
+      <c r="P9" s="63"/>
+      <c r="Q9" s="63"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="63"/>
+      <c r="U9" s="63"/>
+      <c r="V9" s="63"/>
+      <c r="W9" s="63"/>
+      <c r="X9" s="63"/>
+      <c r="Y9" s="63"/>
       <c r="Z9" s="18"/>
       <c r="AA9" s="19"/>
-      <c r="AB9" s="37"/>
-      <c r="AC9" s="37"/>
-      <c r="AD9" s="37"/>
-      <c r="AE9" s="37"/>
-      <c r="AF9" s="37"/>
-      <c r="AG9" s="37"/>
-      <c r="AH9" s="37"/>
-      <c r="AI9" s="37"/>
-      <c r="AJ9" s="37"/>
-      <c r="AK9" s="37"/>
-      <c r="AL9" s="37"/>
-      <c r="AM9" s="38"/>
+      <c r="AB9" s="46"/>
+      <c r="AC9" s="46"/>
+      <c r="AD9" s="46"/>
+      <c r="AE9" s="46"/>
+      <c r="AF9" s="46"/>
+      <c r="AG9" s="46"/>
+      <c r="AH9" s="46"/>
+      <c r="AI9" s="46"/>
+      <c r="AJ9" s="46"/>
+      <c r="AK9" s="46"/>
+      <c r="AL9" s="46"/>
+      <c r="AM9" s="47"/>
       <c r="AQ9" s="21"/>
       <c r="AR9" s="21"/>
       <c r="AS9" s="21"/>
@@ -1818,43 +1818,43 @@
     <row r="10" spans="1:63" s="20" customFormat="1" ht="15.75" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="15"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="54"/>
-      <c r="M10" s="54"/>
-      <c r="N10" s="54"/>
-      <c r="O10" s="54"/>
-      <c r="P10" s="54"/>
-      <c r="Q10" s="54"/>
-      <c r="R10" s="54"/>
-      <c r="S10" s="54"/>
-      <c r="T10" s="54"/>
-      <c r="U10" s="54"/>
-      <c r="V10" s="54"/>
-      <c r="W10" s="54"/>
-      <c r="X10" s="54"/>
-      <c r="Y10" s="54"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="63"/>
+      <c r="P10" s="63"/>
+      <c r="Q10" s="63"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="63"/>
+      <c r="T10" s="63"/>
+      <c r="U10" s="63"/>
+      <c r="V10" s="63"/>
+      <c r="W10" s="63"/>
+      <c r="X10" s="63"/>
+      <c r="Y10" s="63"/>
       <c r="Z10" s="18"/>
       <c r="AA10" s="22"/>
-      <c r="AB10" s="39"/>
-      <c r="AC10" s="39"/>
-      <c r="AD10" s="39"/>
-      <c r="AE10" s="39"/>
-      <c r="AF10" s="40"/>
-      <c r="AG10" s="40"/>
-      <c r="AH10" s="40"/>
-      <c r="AI10" s="40"/>
-      <c r="AJ10" s="40"/>
-      <c r="AK10" s="40"/>
-      <c r="AL10" s="40"/>
-      <c r="AM10" s="41"/>
+      <c r="AB10" s="48"/>
+      <c r="AC10" s="48"/>
+      <c r="AD10" s="48"/>
+      <c r="AE10" s="48"/>
+      <c r="AF10" s="49"/>
+      <c r="AG10" s="49"/>
+      <c r="AH10" s="49"/>
+      <c r="AI10" s="49"/>
+      <c r="AJ10" s="49"/>
+      <c r="AK10" s="49"/>
+      <c r="AL10" s="49"/>
+      <c r="AM10" s="50"/>
       <c r="AQ10" s="21"/>
       <c r="AR10" s="21"/>
       <c r="AS10" s="21"/>
@@ -2045,41 +2045,41 @@
       <c r="A14" s="13"/>
       <c r="B14" s="1"/>
       <c r="C14" s="31"/>
-      <c r="D14" s="59" t="s">
+      <c r="D14" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="59"/>
-      <c r="K14" s="59"/>
-      <c r="L14" s="59"/>
-      <c r="M14" s="59"/>
-      <c r="N14" s="59"/>
-      <c r="O14" s="59"/>
-      <c r="P14" s="59"/>
-      <c r="Q14" s="59"/>
-      <c r="R14" s="59"/>
-      <c r="S14" s="59"/>
-      <c r="T14" s="59"/>
-      <c r="U14" s="59"/>
-      <c r="V14" s="59"/>
-      <c r="W14" s="59"/>
-      <c r="X14" s="59"/>
-      <c r="Y14" s="59"/>
-      <c r="Z14" s="59"/>
-      <c r="AA14" s="59"/>
-      <c r="AB14" s="59"/>
-      <c r="AC14" s="59"/>
-      <c r="AD14" s="59"/>
-      <c r="AE14" s="59"/>
-      <c r="AF14" s="59"/>
-      <c r="AG14" s="59"/>
-      <c r="AH14" s="59"/>
-      <c r="AI14" s="59"/>
-      <c r="AJ14" s="59"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="40"/>
+      <c r="S14" s="40"/>
+      <c r="T14" s="40"/>
+      <c r="U14" s="40"/>
+      <c r="V14" s="40"/>
+      <c r="W14" s="40"/>
+      <c r="X14" s="40"/>
+      <c r="Y14" s="40"/>
+      <c r="Z14" s="40"/>
+      <c r="AA14" s="40"/>
+      <c r="AB14" s="40"/>
+      <c r="AC14" s="40"/>
+      <c r="AD14" s="40"/>
+      <c r="AE14" s="40"/>
+      <c r="AF14" s="40"/>
+      <c r="AG14" s="40"/>
+      <c r="AH14" s="40"/>
+      <c r="AI14" s="40"/>
+      <c r="AJ14" s="40"/>
       <c r="AK14" s="1"/>
       <c r="AL14" s="1"/>
       <c r="AM14" s="12"/>
@@ -2098,39 +2098,39 @@
       <c r="A15" s="13"/>
       <c r="B15" s="32"/>
       <c r="C15" s="31"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="59"/>
-      <c r="O15" s="59"/>
-      <c r="P15" s="59"/>
-      <c r="Q15" s="59"/>
-      <c r="R15" s="59"/>
-      <c r="S15" s="59"/>
-      <c r="T15" s="59"/>
-      <c r="U15" s="59"/>
-      <c r="V15" s="59"/>
-      <c r="W15" s="59"/>
-      <c r="X15" s="59"/>
-      <c r="Y15" s="59"/>
-      <c r="Z15" s="59"/>
-      <c r="AA15" s="59"/>
-      <c r="AB15" s="59"/>
-      <c r="AC15" s="59"/>
-      <c r="AD15" s="59"/>
-      <c r="AE15" s="59"/>
-      <c r="AF15" s="59"/>
-      <c r="AG15" s="59"/>
-      <c r="AH15" s="59"/>
-      <c r="AI15" s="59"/>
-      <c r="AJ15" s="59"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="40"/>
+      <c r="S15" s="40"/>
+      <c r="T15" s="40"/>
+      <c r="U15" s="40"/>
+      <c r="V15" s="40"/>
+      <c r="W15" s="40"/>
+      <c r="X15" s="40"/>
+      <c r="Y15" s="40"/>
+      <c r="Z15" s="40"/>
+      <c r="AA15" s="40"/>
+      <c r="AB15" s="40"/>
+      <c r="AC15" s="40"/>
+      <c r="AD15" s="40"/>
+      <c r="AE15" s="40"/>
+      <c r="AF15" s="40"/>
+      <c r="AG15" s="40"/>
+      <c r="AH15" s="40"/>
+      <c r="AI15" s="40"/>
+      <c r="AJ15" s="40"/>
       <c r="AK15" s="1"/>
       <c r="AL15" s="1"/>
       <c r="AM15" s="12"/>
@@ -2148,55 +2148,55 @@
     <row r="16" spans="1:63" ht="39" customHeight="1">
       <c r="A16" s="13"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="55" t="s">
+      <c r="C16" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55" t="s">
+      <c r="D16" s="37"/>
+      <c r="E16" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55" t="s">
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="55"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="60" t="s">
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="L16" s="61"/>
-      <c r="M16" s="61"/>
-      <c r="N16" s="61"/>
-      <c r="O16" s="61"/>
-      <c r="P16" s="61"/>
-      <c r="Q16" s="61"/>
-      <c r="R16" s="61"/>
-      <c r="S16" s="62"/>
-      <c r="T16" s="63" t="s">
+      <c r="L16" s="42"/>
+      <c r="M16" s="42"/>
+      <c r="N16" s="42"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="42"/>
+      <c r="Q16" s="42"/>
+      <c r="R16" s="42"/>
+      <c r="S16" s="43"/>
+      <c r="T16" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="U16" s="63"/>
-      <c r="V16" s="63"/>
-      <c r="W16" s="63"/>
-      <c r="X16" s="63"/>
-      <c r="Y16" s="63"/>
-      <c r="Z16" s="63"/>
-      <c r="AA16" s="63" t="s">
+      <c r="U16" s="44"/>
+      <c r="V16" s="44"/>
+      <c r="W16" s="44"/>
+      <c r="X16" s="44"/>
+      <c r="Y16" s="44"/>
+      <c r="Z16" s="44"/>
+      <c r="AA16" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="AB16" s="63"/>
-      <c r="AC16" s="63"/>
-      <c r="AD16" s="63"/>
-      <c r="AE16" s="63"/>
-      <c r="AF16" s="63"/>
-      <c r="AG16" s="63"/>
-      <c r="AH16" s="63"/>
-      <c r="AI16" s="63"/>
-      <c r="AJ16" s="63"/>
-      <c r="AK16" s="63"/>
-      <c r="AL16" s="63"/>
-      <c r="AM16" s="64"/>
+      <c r="AB16" s="44"/>
+      <c r="AC16" s="44"/>
+      <c r="AD16" s="44"/>
+      <c r="AE16" s="44"/>
+      <c r="AF16" s="44"/>
+      <c r="AG16" s="44"/>
+      <c r="AH16" s="44"/>
+      <c r="AI16" s="44"/>
+      <c r="AJ16" s="44"/>
+      <c r="AK16" s="44"/>
+      <c r="AL16" s="44"/>
+      <c r="AM16" s="45"/>
       <c r="AN16" s="1"/>
       <c r="AO16" s="1"/>
       <c r="AP16" s="1"/>
@@ -2211,43 +2211,43 @@
     <row r="17" spans="1:49" ht="45" customHeight="1">
       <c r="A17" s="13"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="56"/>
-      <c r="L17" s="56"/>
-      <c r="M17" s="56"/>
-      <c r="N17" s="56"/>
-      <c r="O17" s="56"/>
-      <c r="P17" s="56"/>
-      <c r="Q17" s="56"/>
-      <c r="R17" s="56"/>
-      <c r="S17" s="56"/>
-      <c r="T17" s="56"/>
-      <c r="U17" s="56"/>
-      <c r="V17" s="56"/>
-      <c r="W17" s="56"/>
-      <c r="X17" s="56"/>
-      <c r="Y17" s="56"/>
-      <c r="Z17" s="56"/>
-      <c r="AA17" s="57"/>
-      <c r="AB17" s="57"/>
-      <c r="AC17" s="57"/>
-      <c r="AD17" s="57"/>
-      <c r="AE17" s="57"/>
-      <c r="AF17" s="57"/>
-      <c r="AG17" s="57"/>
-      <c r="AH17" s="57"/>
-      <c r="AI17" s="57"/>
-      <c r="AJ17" s="57"/>
-      <c r="AK17" s="57"/>
-      <c r="AL17" s="57"/>
-      <c r="AM17" s="58"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="64"/>
+      <c r="M17" s="64"/>
+      <c r="N17" s="64"/>
+      <c r="O17" s="64"/>
+      <c r="P17" s="64"/>
+      <c r="Q17" s="64"/>
+      <c r="R17" s="64"/>
+      <c r="S17" s="64"/>
+      <c r="T17" s="64"/>
+      <c r="U17" s="64"/>
+      <c r="V17" s="64"/>
+      <c r="W17" s="64"/>
+      <c r="X17" s="64"/>
+      <c r="Y17" s="64"/>
+      <c r="Z17" s="64"/>
+      <c r="AA17" s="65"/>
+      <c r="AB17" s="65"/>
+      <c r="AC17" s="65"/>
+      <c r="AD17" s="65"/>
+      <c r="AE17" s="65"/>
+      <c r="AF17" s="65"/>
+      <c r="AG17" s="65"/>
+      <c r="AH17" s="65"/>
+      <c r="AI17" s="65"/>
+      <c r="AJ17" s="65"/>
+      <c r="AK17" s="65"/>
+      <c r="AL17" s="65"/>
+      <c r="AM17" s="66"/>
       <c r="AN17" s="1"/>
       <c r="AO17" s="1"/>
       <c r="AP17" s="1"/>
@@ -2262,43 +2262,43 @@
     <row r="18" spans="1:49" ht="45" customHeight="1">
       <c r="A18" s="13"/>
       <c r="B18" s="33"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="56"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="56"/>
-      <c r="O18" s="56"/>
-      <c r="P18" s="56"/>
-      <c r="Q18" s="56"/>
-      <c r="R18" s="56"/>
-      <c r="S18" s="56"/>
-      <c r="T18" s="56"/>
-      <c r="U18" s="56"/>
-      <c r="V18" s="56"/>
-      <c r="W18" s="56"/>
-      <c r="X18" s="56"/>
-      <c r="Y18" s="56"/>
-      <c r="Z18" s="56"/>
-      <c r="AA18" s="57"/>
-      <c r="AB18" s="57"/>
-      <c r="AC18" s="57"/>
-      <c r="AD18" s="57"/>
-      <c r="AE18" s="57"/>
-      <c r="AF18" s="57"/>
-      <c r="AG18" s="57"/>
-      <c r="AH18" s="57"/>
-      <c r="AI18" s="57"/>
-      <c r="AJ18" s="57"/>
-      <c r="AK18" s="57"/>
-      <c r="AL18" s="57"/>
-      <c r="AM18" s="58"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="64"/>
+      <c r="L18" s="64"/>
+      <c r="M18" s="64"/>
+      <c r="N18" s="64"/>
+      <c r="O18" s="64"/>
+      <c r="P18" s="64"/>
+      <c r="Q18" s="64"/>
+      <c r="R18" s="64"/>
+      <c r="S18" s="64"/>
+      <c r="T18" s="64"/>
+      <c r="U18" s="64"/>
+      <c r="V18" s="64"/>
+      <c r="W18" s="64"/>
+      <c r="X18" s="64"/>
+      <c r="Y18" s="64"/>
+      <c r="Z18" s="64"/>
+      <c r="AA18" s="65"/>
+      <c r="AB18" s="65"/>
+      <c r="AC18" s="65"/>
+      <c r="AD18" s="65"/>
+      <c r="AE18" s="65"/>
+      <c r="AF18" s="65"/>
+      <c r="AG18" s="65"/>
+      <c r="AH18" s="65"/>
+      <c r="AI18" s="65"/>
+      <c r="AJ18" s="65"/>
+      <c r="AK18" s="65"/>
+      <c r="AL18" s="65"/>
+      <c r="AM18" s="66"/>
       <c r="AN18" s="1"/>
       <c r="AO18" s="1"/>
       <c r="AP18" s="1"/>
@@ -2313,43 +2313,43 @@
     <row r="19" spans="1:49" ht="45" customHeight="1">
       <c r="A19" s="13"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="55"/>
-      <c r="J19" s="55"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="56"/>
-      <c r="M19" s="56"/>
-      <c r="N19" s="56"/>
-      <c r="O19" s="56"/>
-      <c r="P19" s="56"/>
-      <c r="Q19" s="56"/>
-      <c r="R19" s="56"/>
-      <c r="S19" s="56"/>
-      <c r="T19" s="56"/>
-      <c r="U19" s="56"/>
-      <c r="V19" s="56"/>
-      <c r="W19" s="56"/>
-      <c r="X19" s="56"/>
-      <c r="Y19" s="56"/>
-      <c r="Z19" s="56"/>
-      <c r="AA19" s="57"/>
-      <c r="AB19" s="57"/>
-      <c r="AC19" s="57"/>
-      <c r="AD19" s="57"/>
-      <c r="AE19" s="57"/>
-      <c r="AF19" s="57"/>
-      <c r="AG19" s="57"/>
-      <c r="AH19" s="57"/>
-      <c r="AI19" s="57"/>
-      <c r="AJ19" s="57"/>
-      <c r="AK19" s="57"/>
-      <c r="AL19" s="57"/>
-      <c r="AM19" s="58"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="64"/>
+      <c r="L19" s="64"/>
+      <c r="M19" s="64"/>
+      <c r="N19" s="64"/>
+      <c r="O19" s="64"/>
+      <c r="P19" s="64"/>
+      <c r="Q19" s="64"/>
+      <c r="R19" s="64"/>
+      <c r="S19" s="64"/>
+      <c r="T19" s="64"/>
+      <c r="U19" s="64"/>
+      <c r="V19" s="64"/>
+      <c r="W19" s="64"/>
+      <c r="X19" s="64"/>
+      <c r="Y19" s="64"/>
+      <c r="Z19" s="64"/>
+      <c r="AA19" s="65"/>
+      <c r="AB19" s="65"/>
+      <c r="AC19" s="65"/>
+      <c r="AD19" s="65"/>
+      <c r="AE19" s="65"/>
+      <c r="AF19" s="65"/>
+      <c r="AG19" s="65"/>
+      <c r="AH19" s="65"/>
+      <c r="AI19" s="65"/>
+      <c r="AJ19" s="65"/>
+      <c r="AK19" s="65"/>
+      <c r="AL19" s="65"/>
+      <c r="AM19" s="66"/>
       <c r="AN19" s="1"/>
       <c r="AO19" s="1"/>
       <c r="AP19" s="1"/>
@@ -2364,43 +2364,43 @@
     <row r="20" spans="1:49" ht="45" customHeight="1">
       <c r="A20" s="13"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="55"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="56"/>
-      <c r="O20" s="56"/>
-      <c r="P20" s="56"/>
-      <c r="Q20" s="56"/>
-      <c r="R20" s="56"/>
-      <c r="S20" s="56"/>
-      <c r="T20" s="56"/>
-      <c r="U20" s="56"/>
-      <c r="V20" s="56"/>
-      <c r="W20" s="56"/>
-      <c r="X20" s="56"/>
-      <c r="Y20" s="56"/>
-      <c r="Z20" s="56"/>
-      <c r="AA20" s="57"/>
-      <c r="AB20" s="57"/>
-      <c r="AC20" s="57"/>
-      <c r="AD20" s="57"/>
-      <c r="AE20" s="57"/>
-      <c r="AF20" s="57"/>
-      <c r="AG20" s="57"/>
-      <c r="AH20" s="57"/>
-      <c r="AI20" s="57"/>
-      <c r="AJ20" s="57"/>
-      <c r="AK20" s="57"/>
-      <c r="AL20" s="57"/>
-      <c r="AM20" s="58"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="64"/>
+      <c r="L20" s="64"/>
+      <c r="M20" s="64"/>
+      <c r="N20" s="64"/>
+      <c r="O20" s="64"/>
+      <c r="P20" s="64"/>
+      <c r="Q20" s="64"/>
+      <c r="R20" s="64"/>
+      <c r="S20" s="64"/>
+      <c r="T20" s="64"/>
+      <c r="U20" s="64"/>
+      <c r="V20" s="64"/>
+      <c r="W20" s="64"/>
+      <c r="X20" s="64"/>
+      <c r="Y20" s="64"/>
+      <c r="Z20" s="64"/>
+      <c r="AA20" s="65"/>
+      <c r="AB20" s="65"/>
+      <c r="AC20" s="65"/>
+      <c r="AD20" s="65"/>
+      <c r="AE20" s="65"/>
+      <c r="AF20" s="65"/>
+      <c r="AG20" s="65"/>
+      <c r="AH20" s="65"/>
+      <c r="AI20" s="65"/>
+      <c r="AJ20" s="65"/>
+      <c r="AK20" s="65"/>
+      <c r="AL20" s="65"/>
+      <c r="AM20" s="66"/>
       <c r="AN20" s="1"/>
       <c r="AO20" s="1"/>
       <c r="AP20" s="1"/>
@@ -2415,43 +2415,43 @@
     <row r="21" spans="1:49" ht="45" customHeight="1">
       <c r="A21" s="13"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="55"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="56"/>
-      <c r="M21" s="56"/>
-      <c r="N21" s="56"/>
-      <c r="O21" s="56"/>
-      <c r="P21" s="56"/>
-      <c r="Q21" s="56"/>
-      <c r="R21" s="56"/>
-      <c r="S21" s="56"/>
-      <c r="T21" s="56"/>
-      <c r="U21" s="56"/>
-      <c r="V21" s="56"/>
-      <c r="W21" s="56"/>
-      <c r="X21" s="56"/>
-      <c r="Y21" s="56"/>
-      <c r="Z21" s="56"/>
-      <c r="AA21" s="57"/>
-      <c r="AB21" s="57"/>
-      <c r="AC21" s="57"/>
-      <c r="AD21" s="57"/>
-      <c r="AE21" s="57"/>
-      <c r="AF21" s="57"/>
-      <c r="AG21" s="57"/>
-      <c r="AH21" s="57"/>
-      <c r="AI21" s="57"/>
-      <c r="AJ21" s="57"/>
-      <c r="AK21" s="57"/>
-      <c r="AL21" s="57"/>
-      <c r="AM21" s="58"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="64"/>
+      <c r="M21" s="64"/>
+      <c r="N21" s="64"/>
+      <c r="O21" s="64"/>
+      <c r="P21" s="64"/>
+      <c r="Q21" s="64"/>
+      <c r="R21" s="64"/>
+      <c r="S21" s="64"/>
+      <c r="T21" s="64"/>
+      <c r="U21" s="64"/>
+      <c r="V21" s="64"/>
+      <c r="W21" s="64"/>
+      <c r="X21" s="64"/>
+      <c r="Y21" s="64"/>
+      <c r="Z21" s="64"/>
+      <c r="AA21" s="65"/>
+      <c r="AB21" s="65"/>
+      <c r="AC21" s="65"/>
+      <c r="AD21" s="65"/>
+      <c r="AE21" s="65"/>
+      <c r="AF21" s="65"/>
+      <c r="AG21" s="65"/>
+      <c r="AH21" s="65"/>
+      <c r="AI21" s="65"/>
+      <c r="AJ21" s="65"/>
+      <c r="AK21" s="65"/>
+      <c r="AL21" s="65"/>
+      <c r="AM21" s="66"/>
       <c r="AN21" s="1"/>
       <c r="AO21" s="1"/>
       <c r="AP21" s="1"/>
@@ -2466,43 +2466,43 @@
     <row r="22" spans="1:49" ht="45" customHeight="1">
       <c r="A22" s="13"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="55"/>
-      <c r="J22" s="55"/>
-      <c r="K22" s="56"/>
-      <c r="L22" s="56"/>
-      <c r="M22" s="56"/>
-      <c r="N22" s="56"/>
-      <c r="O22" s="56"/>
-      <c r="P22" s="56"/>
-      <c r="Q22" s="56"/>
-      <c r="R22" s="56"/>
-      <c r="S22" s="56"/>
-      <c r="T22" s="56"/>
-      <c r="U22" s="56"/>
-      <c r="V22" s="56"/>
-      <c r="W22" s="56"/>
-      <c r="X22" s="56"/>
-      <c r="Y22" s="56"/>
-      <c r="Z22" s="56"/>
-      <c r="AA22" s="57"/>
-      <c r="AB22" s="57"/>
-      <c r="AC22" s="57"/>
-      <c r="AD22" s="57"/>
-      <c r="AE22" s="57"/>
-      <c r="AF22" s="57"/>
-      <c r="AG22" s="57"/>
-      <c r="AH22" s="57"/>
-      <c r="AI22" s="57"/>
-      <c r="AJ22" s="57"/>
-      <c r="AK22" s="57"/>
-      <c r="AL22" s="57"/>
-      <c r="AM22" s="58"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="64"/>
+      <c r="M22" s="64"/>
+      <c r="N22" s="64"/>
+      <c r="O22" s="64"/>
+      <c r="P22" s="64"/>
+      <c r="Q22" s="64"/>
+      <c r="R22" s="64"/>
+      <c r="S22" s="64"/>
+      <c r="T22" s="64"/>
+      <c r="U22" s="64"/>
+      <c r="V22" s="64"/>
+      <c r="W22" s="64"/>
+      <c r="X22" s="64"/>
+      <c r="Y22" s="64"/>
+      <c r="Z22" s="64"/>
+      <c r="AA22" s="65"/>
+      <c r="AB22" s="65"/>
+      <c r="AC22" s="65"/>
+      <c r="AD22" s="65"/>
+      <c r="AE22" s="65"/>
+      <c r="AF22" s="65"/>
+      <c r="AG22" s="65"/>
+      <c r="AH22" s="65"/>
+      <c r="AI22" s="65"/>
+      <c r="AJ22" s="65"/>
+      <c r="AK22" s="65"/>
+      <c r="AL22" s="65"/>
+      <c r="AM22" s="66"/>
       <c r="AN22" s="1"/>
       <c r="AO22" s="1"/>
       <c r="AP22" s="1"/>
@@ -2517,43 +2517,43 @@
     <row r="23" spans="1:49" ht="45" customHeight="1">
       <c r="A23" s="13"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="55"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="56"/>
-      <c r="L23" s="56"/>
-      <c r="M23" s="56"/>
-      <c r="N23" s="56"/>
-      <c r="O23" s="56"/>
-      <c r="P23" s="56"/>
-      <c r="Q23" s="56"/>
-      <c r="R23" s="56"/>
-      <c r="S23" s="56"/>
-      <c r="T23" s="56"/>
-      <c r="U23" s="56"/>
-      <c r="V23" s="56"/>
-      <c r="W23" s="56"/>
-      <c r="X23" s="56"/>
-      <c r="Y23" s="56"/>
-      <c r="Z23" s="56"/>
-      <c r="AA23" s="57"/>
-      <c r="AB23" s="57"/>
-      <c r="AC23" s="57"/>
-      <c r="AD23" s="57"/>
-      <c r="AE23" s="57"/>
-      <c r="AF23" s="57"/>
-      <c r="AG23" s="57"/>
-      <c r="AH23" s="57"/>
-      <c r="AI23" s="57"/>
-      <c r="AJ23" s="57"/>
-      <c r="AK23" s="57"/>
-      <c r="AL23" s="57"/>
-      <c r="AM23" s="58"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="64"/>
+      <c r="M23" s="64"/>
+      <c r="N23" s="64"/>
+      <c r="O23" s="64"/>
+      <c r="P23" s="64"/>
+      <c r="Q23" s="64"/>
+      <c r="R23" s="64"/>
+      <c r="S23" s="64"/>
+      <c r="T23" s="64"/>
+      <c r="U23" s="64"/>
+      <c r="V23" s="64"/>
+      <c r="W23" s="64"/>
+      <c r="X23" s="64"/>
+      <c r="Y23" s="64"/>
+      <c r="Z23" s="64"/>
+      <c r="AA23" s="65"/>
+      <c r="AB23" s="65"/>
+      <c r="AC23" s="65"/>
+      <c r="AD23" s="65"/>
+      <c r="AE23" s="65"/>
+      <c r="AF23" s="65"/>
+      <c r="AG23" s="65"/>
+      <c r="AH23" s="65"/>
+      <c r="AI23" s="65"/>
+      <c r="AJ23" s="65"/>
+      <c r="AK23" s="65"/>
+      <c r="AL23" s="65"/>
+      <c r="AM23" s="66"/>
       <c r="AN23" s="1"/>
       <c r="AO23" s="1"/>
       <c r="AP23" s="1"/>
@@ -2568,301 +2568,301 @@
     <row r="24" spans="1:49" ht="45" customHeight="1">
       <c r="A24" s="13"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="55"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="56"/>
-      <c r="L24" s="56"/>
-      <c r="M24" s="56"/>
-      <c r="N24" s="56"/>
-      <c r="O24" s="56"/>
-      <c r="P24" s="56"/>
-      <c r="Q24" s="56"/>
-      <c r="R24" s="56"/>
-      <c r="S24" s="56"/>
-      <c r="T24" s="56"/>
-      <c r="U24" s="56"/>
-      <c r="V24" s="56"/>
-      <c r="W24" s="56"/>
-      <c r="X24" s="56"/>
-      <c r="Y24" s="56"/>
-      <c r="Z24" s="56"/>
-      <c r="AA24" s="57"/>
-      <c r="AB24" s="57"/>
-      <c r="AC24" s="57"/>
-      <c r="AD24" s="57"/>
-      <c r="AE24" s="57"/>
-      <c r="AF24" s="57"/>
-      <c r="AG24" s="57"/>
-      <c r="AH24" s="57"/>
-      <c r="AI24" s="57"/>
-      <c r="AJ24" s="57"/>
-      <c r="AK24" s="57"/>
-      <c r="AL24" s="57"/>
-      <c r="AM24" s="58"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="64"/>
+      <c r="M24" s="64"/>
+      <c r="N24" s="64"/>
+      <c r="O24" s="64"/>
+      <c r="P24" s="64"/>
+      <c r="Q24" s="64"/>
+      <c r="R24" s="64"/>
+      <c r="S24" s="64"/>
+      <c r="T24" s="64"/>
+      <c r="U24" s="64"/>
+      <c r="V24" s="64"/>
+      <c r="W24" s="64"/>
+      <c r="X24" s="64"/>
+      <c r="Y24" s="64"/>
+      <c r="Z24" s="64"/>
+      <c r="AA24" s="65"/>
+      <c r="AB24" s="65"/>
+      <c r="AC24" s="65"/>
+      <c r="AD24" s="65"/>
+      <c r="AE24" s="65"/>
+      <c r="AF24" s="65"/>
+      <c r="AG24" s="65"/>
+      <c r="AH24" s="65"/>
+      <c r="AI24" s="65"/>
+      <c r="AJ24" s="65"/>
+      <c r="AK24" s="65"/>
+      <c r="AL24" s="65"/>
+      <c r="AM24" s="66"/>
     </row>
     <row r="25" spans="1:49" ht="45" customHeight="1">
       <c r="A25" s="13"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="55"/>
-      <c r="K25" s="56"/>
-      <c r="L25" s="56"/>
-      <c r="M25" s="56"/>
-      <c r="N25" s="56"/>
-      <c r="O25" s="56"/>
-      <c r="P25" s="56"/>
-      <c r="Q25" s="56"/>
-      <c r="R25" s="56"/>
-      <c r="S25" s="56"/>
-      <c r="T25" s="56"/>
-      <c r="U25" s="56"/>
-      <c r="V25" s="56"/>
-      <c r="W25" s="56"/>
-      <c r="X25" s="56"/>
-      <c r="Y25" s="56"/>
-      <c r="Z25" s="56"/>
-      <c r="AA25" s="57"/>
-      <c r="AB25" s="57"/>
-      <c r="AC25" s="57"/>
-      <c r="AD25" s="57"/>
-      <c r="AE25" s="57"/>
-      <c r="AF25" s="57"/>
-      <c r="AG25" s="57"/>
-      <c r="AH25" s="57"/>
-      <c r="AI25" s="57"/>
-      <c r="AJ25" s="57"/>
-      <c r="AK25" s="57"/>
-      <c r="AL25" s="57"/>
-      <c r="AM25" s="58"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="64"/>
+      <c r="L25" s="64"/>
+      <c r="M25" s="64"/>
+      <c r="N25" s="64"/>
+      <c r="O25" s="64"/>
+      <c r="P25" s="64"/>
+      <c r="Q25" s="64"/>
+      <c r="R25" s="64"/>
+      <c r="S25" s="64"/>
+      <c r="T25" s="64"/>
+      <c r="U25" s="64"/>
+      <c r="V25" s="64"/>
+      <c r="W25" s="64"/>
+      <c r="X25" s="64"/>
+      <c r="Y25" s="64"/>
+      <c r="Z25" s="64"/>
+      <c r="AA25" s="65"/>
+      <c r="AB25" s="65"/>
+      <c r="AC25" s="65"/>
+      <c r="AD25" s="65"/>
+      <c r="AE25" s="65"/>
+      <c r="AF25" s="65"/>
+      <c r="AG25" s="65"/>
+      <c r="AH25" s="65"/>
+      <c r="AI25" s="65"/>
+      <c r="AJ25" s="65"/>
+      <c r="AK25" s="65"/>
+      <c r="AL25" s="65"/>
+      <c r="AM25" s="66"/>
     </row>
     <row r="26" spans="1:49" ht="45" customHeight="1">
       <c r="A26" s="13"/>
       <c r="B26" s="20"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="56"/>
-      <c r="L26" s="56"/>
-      <c r="M26" s="56"/>
-      <c r="N26" s="56"/>
-      <c r="O26" s="56"/>
-      <c r="P26" s="56"/>
-      <c r="Q26" s="56"/>
-      <c r="R26" s="56"/>
-      <c r="S26" s="56"/>
-      <c r="T26" s="56"/>
-      <c r="U26" s="56"/>
-      <c r="V26" s="56"/>
-      <c r="W26" s="56"/>
-      <c r="X26" s="56"/>
-      <c r="Y26" s="56"/>
-      <c r="Z26" s="56"/>
-      <c r="AA26" s="57"/>
-      <c r="AB26" s="57"/>
-      <c r="AC26" s="57"/>
-      <c r="AD26" s="57"/>
-      <c r="AE26" s="57"/>
-      <c r="AF26" s="57"/>
-      <c r="AG26" s="57"/>
-      <c r="AH26" s="57"/>
-      <c r="AI26" s="57"/>
-      <c r="AJ26" s="57"/>
-      <c r="AK26" s="57"/>
-      <c r="AL26" s="57"/>
-      <c r="AM26" s="58"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="64"/>
+      <c r="L26" s="64"/>
+      <c r="M26" s="64"/>
+      <c r="N26" s="64"/>
+      <c r="O26" s="64"/>
+      <c r="P26" s="64"/>
+      <c r="Q26" s="64"/>
+      <c r="R26" s="64"/>
+      <c r="S26" s="64"/>
+      <c r="T26" s="64"/>
+      <c r="U26" s="64"/>
+      <c r="V26" s="64"/>
+      <c r="W26" s="64"/>
+      <c r="X26" s="64"/>
+      <c r="Y26" s="64"/>
+      <c r="Z26" s="64"/>
+      <c r="AA26" s="65"/>
+      <c r="AB26" s="65"/>
+      <c r="AC26" s="65"/>
+      <c r="AD26" s="65"/>
+      <c r="AE26" s="65"/>
+      <c r="AF26" s="65"/>
+      <c r="AG26" s="65"/>
+      <c r="AH26" s="65"/>
+      <c r="AI26" s="65"/>
+      <c r="AJ26" s="65"/>
+      <c r="AK26" s="65"/>
+      <c r="AL26" s="65"/>
+      <c r="AM26" s="66"/>
     </row>
     <row r="27" spans="1:49" ht="45" customHeight="1">
       <c r="A27" s="13"/>
       <c r="B27" s="20"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="55"/>
-      <c r="K27" s="56"/>
-      <c r="L27" s="56"/>
-      <c r="M27" s="56"/>
-      <c r="N27" s="56"/>
-      <c r="O27" s="56"/>
-      <c r="P27" s="56"/>
-      <c r="Q27" s="56"/>
-      <c r="R27" s="56"/>
-      <c r="S27" s="56"/>
-      <c r="T27" s="56"/>
-      <c r="U27" s="56"/>
-      <c r="V27" s="56"/>
-      <c r="W27" s="56"/>
-      <c r="X27" s="56"/>
-      <c r="Y27" s="56"/>
-      <c r="Z27" s="56"/>
-      <c r="AA27" s="57"/>
-      <c r="AB27" s="57"/>
-      <c r="AC27" s="57"/>
-      <c r="AD27" s="57"/>
-      <c r="AE27" s="57"/>
-      <c r="AF27" s="57"/>
-      <c r="AG27" s="57"/>
-      <c r="AH27" s="57"/>
-      <c r="AI27" s="57"/>
-      <c r="AJ27" s="57"/>
-      <c r="AK27" s="57"/>
-      <c r="AL27" s="57"/>
-      <c r="AM27" s="58"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="64"/>
+      <c r="L27" s="64"/>
+      <c r="M27" s="64"/>
+      <c r="N27" s="64"/>
+      <c r="O27" s="64"/>
+      <c r="P27" s="64"/>
+      <c r="Q27" s="64"/>
+      <c r="R27" s="64"/>
+      <c r="S27" s="64"/>
+      <c r="T27" s="64"/>
+      <c r="U27" s="64"/>
+      <c r="V27" s="64"/>
+      <c r="W27" s="64"/>
+      <c r="X27" s="64"/>
+      <c r="Y27" s="64"/>
+      <c r="Z27" s="64"/>
+      <c r="AA27" s="65"/>
+      <c r="AB27" s="65"/>
+      <c r="AC27" s="65"/>
+      <c r="AD27" s="65"/>
+      <c r="AE27" s="65"/>
+      <c r="AF27" s="65"/>
+      <c r="AG27" s="65"/>
+      <c r="AH27" s="65"/>
+      <c r="AI27" s="65"/>
+      <c r="AJ27" s="65"/>
+      <c r="AK27" s="65"/>
+      <c r="AL27" s="65"/>
+      <c r="AM27" s="66"/>
     </row>
     <row r="28" spans="1:49" ht="45" customHeight="1">
       <c r="A28" s="13"/>
       <c r="B28" s="20"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="65"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="66"/>
-      <c r="L28" s="66"/>
-      <c r="M28" s="66"/>
-      <c r="N28" s="66"/>
-      <c r="O28" s="66"/>
-      <c r="P28" s="66"/>
-      <c r="Q28" s="66"/>
-      <c r="R28" s="66"/>
-      <c r="S28" s="66"/>
-      <c r="T28" s="66"/>
-      <c r="U28" s="66"/>
-      <c r="V28" s="66"/>
-      <c r="W28" s="66"/>
-      <c r="X28" s="66"/>
-      <c r="Y28" s="66"/>
-      <c r="Z28" s="66"/>
-      <c r="AA28" s="67"/>
-      <c r="AB28" s="67"/>
-      <c r="AC28" s="67"/>
-      <c r="AD28" s="67"/>
-      <c r="AE28" s="67"/>
-      <c r="AF28" s="67"/>
-      <c r="AG28" s="67"/>
-      <c r="AH28" s="67"/>
-      <c r="AI28" s="67"/>
-      <c r="AJ28" s="67"/>
-      <c r="AK28" s="67"/>
-      <c r="AL28" s="67"/>
-      <c r="AM28" s="68"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="67"/>
+      <c r="M28" s="67"/>
+      <c r="N28" s="67"/>
+      <c r="O28" s="67"/>
+      <c r="P28" s="67"/>
+      <c r="Q28" s="67"/>
+      <c r="R28" s="67"/>
+      <c r="S28" s="67"/>
+      <c r="T28" s="67"/>
+      <c r="U28" s="67"/>
+      <c r="V28" s="67"/>
+      <c r="W28" s="67"/>
+      <c r="X28" s="67"/>
+      <c r="Y28" s="67"/>
+      <c r="Z28" s="67"/>
+      <c r="AA28" s="68"/>
+      <c r="AB28" s="68"/>
+      <c r="AC28" s="68"/>
+      <c r="AD28" s="68"/>
+      <c r="AE28" s="68"/>
+      <c r="AF28" s="68"/>
+      <c r="AG28" s="68"/>
+      <c r="AH28" s="68"/>
+      <c r="AI28" s="68"/>
+      <c r="AJ28" s="68"/>
+      <c r="AK28" s="68"/>
+      <c r="AL28" s="68"/>
+      <c r="AM28" s="69"/>
     </row>
     <row r="29" spans="1:49" ht="45" customHeight="1">
       <c r="A29" s="13"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
-      <c r="K29" s="56"/>
-      <c r="L29" s="56"/>
-      <c r="M29" s="56"/>
-      <c r="N29" s="56"/>
-      <c r="O29" s="56"/>
-      <c r="P29" s="56"/>
-      <c r="Q29" s="56"/>
-      <c r="R29" s="56"/>
-      <c r="S29" s="56"/>
-      <c r="T29" s="56"/>
-      <c r="U29" s="56"/>
-      <c r="V29" s="56"/>
-      <c r="W29" s="56"/>
-      <c r="X29" s="56"/>
-      <c r="Y29" s="56"/>
-      <c r="Z29" s="56"/>
-      <c r="AA29" s="57"/>
-      <c r="AB29" s="57"/>
-      <c r="AC29" s="57"/>
-      <c r="AD29" s="57"/>
-      <c r="AE29" s="57"/>
-      <c r="AF29" s="57"/>
-      <c r="AG29" s="57"/>
-      <c r="AH29" s="57"/>
-      <c r="AI29" s="57"/>
-      <c r="AJ29" s="57"/>
-      <c r="AK29" s="57"/>
-      <c r="AL29" s="57"/>
-      <c r="AM29" s="58"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="64"/>
+      <c r="L29" s="64"/>
+      <c r="M29" s="64"/>
+      <c r="N29" s="64"/>
+      <c r="O29" s="64"/>
+      <c r="P29" s="64"/>
+      <c r="Q29" s="64"/>
+      <c r="R29" s="64"/>
+      <c r="S29" s="64"/>
+      <c r="T29" s="64"/>
+      <c r="U29" s="64"/>
+      <c r="V29" s="64"/>
+      <c r="W29" s="64"/>
+      <c r="X29" s="64"/>
+      <c r="Y29" s="64"/>
+      <c r="Z29" s="64"/>
+      <c r="AA29" s="65"/>
+      <c r="AB29" s="65"/>
+      <c r="AC29" s="65"/>
+      <c r="AD29" s="65"/>
+      <c r="AE29" s="65"/>
+      <c r="AF29" s="65"/>
+      <c r="AG29" s="65"/>
+      <c r="AH29" s="65"/>
+      <c r="AI29" s="65"/>
+      <c r="AJ29" s="65"/>
+      <c r="AK29" s="65"/>
+      <c r="AL29" s="65"/>
+      <c r="AM29" s="66"/>
     </row>
     <row r="30" spans="1:49" ht="45" customHeight="1">
       <c r="A30" s="13"/>
       <c r="B30" s="20"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="55"/>
-      <c r="J30" s="55"/>
-      <c r="K30" s="56"/>
-      <c r="L30" s="56"/>
-      <c r="M30" s="56"/>
-      <c r="N30" s="56"/>
-      <c r="O30" s="56"/>
-      <c r="P30" s="56"/>
-      <c r="Q30" s="56"/>
-      <c r="R30" s="56"/>
-      <c r="S30" s="56"/>
-      <c r="T30" s="56"/>
-      <c r="U30" s="56"/>
-      <c r="V30" s="56"/>
-      <c r="W30" s="56"/>
-      <c r="X30" s="56"/>
-      <c r="Y30" s="56"/>
-      <c r="Z30" s="56"/>
-      <c r="AA30" s="57"/>
-      <c r="AB30" s="57"/>
-      <c r="AC30" s="57"/>
-      <c r="AD30" s="57"/>
-      <c r="AE30" s="57"/>
-      <c r="AF30" s="57"/>
-      <c r="AG30" s="57"/>
-      <c r="AH30" s="57"/>
-      <c r="AI30" s="57"/>
-      <c r="AJ30" s="57"/>
-      <c r="AK30" s="57"/>
-      <c r="AL30" s="57"/>
-      <c r="AM30" s="58"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="64"/>
+      <c r="L30" s="64"/>
+      <c r="M30" s="64"/>
+      <c r="N30" s="64"/>
+      <c r="O30" s="64"/>
+      <c r="P30" s="64"/>
+      <c r="Q30" s="64"/>
+      <c r="R30" s="64"/>
+      <c r="S30" s="64"/>
+      <c r="T30" s="64"/>
+      <c r="U30" s="64"/>
+      <c r="V30" s="64"/>
+      <c r="W30" s="64"/>
+      <c r="X30" s="64"/>
+      <c r="Y30" s="64"/>
+      <c r="Z30" s="64"/>
+      <c r="AA30" s="65"/>
+      <c r="AB30" s="65"/>
+      <c r="AC30" s="65"/>
+      <c r="AD30" s="65"/>
+      <c r="AE30" s="65"/>
+      <c r="AF30" s="65"/>
+      <c r="AG30" s="65"/>
+      <c r="AH30" s="65"/>
+      <c r="AI30" s="65"/>
+      <c r="AJ30" s="65"/>
+      <c r="AK30" s="65"/>
+      <c r="AL30" s="65"/>
+      <c r="AM30" s="66"/>
     </row>
     <row r="31" spans="1:49" ht="45" customHeight="1" thickBot="1">
       <c r="A31" s="34"/>
       <c r="B31" s="35"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="69"/>
-      <c r="F31" s="69"/>
-      <c r="G31" s="69"/>
-      <c r="H31" s="55"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="55"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="37"/>
       <c r="K31" s="70"/>
       <c r="L31" s="70"/>
       <c r="M31" s="70"/>
@@ -2895,103 +2895,6 @@
     </row>
   </sheetData>
   <mergeCells count="111">
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="K31:S31"/>
-    <mergeCell ref="T31:Z31"/>
-    <mergeCell ref="AA31:AM31"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="H30:J30"/>
-    <mergeCell ref="K30:S30"/>
-    <mergeCell ref="T30:Z30"/>
-    <mergeCell ref="AA30:AM30"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="K29:S29"/>
-    <mergeCell ref="T29:Z29"/>
-    <mergeCell ref="AA29:AM29"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="H28:J28"/>
-    <mergeCell ref="K28:S28"/>
-    <mergeCell ref="T28:Z28"/>
-    <mergeCell ref="AA28:AM28"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="K27:S27"/>
-    <mergeCell ref="T27:Z27"/>
-    <mergeCell ref="AA27:AM27"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="K26:S26"/>
-    <mergeCell ref="T26:Z26"/>
-    <mergeCell ref="AA26:AM26"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="K25:S25"/>
-    <mergeCell ref="T25:Z25"/>
-    <mergeCell ref="AA25:AM25"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="K24:S24"/>
-    <mergeCell ref="T24:Z24"/>
-    <mergeCell ref="AA24:AM24"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:S23"/>
-    <mergeCell ref="T23:Z23"/>
-    <mergeCell ref="AA23:AM23"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:S22"/>
-    <mergeCell ref="T22:Z22"/>
-    <mergeCell ref="AA22:AM22"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K21:S21"/>
-    <mergeCell ref="T21:Z21"/>
-    <mergeCell ref="AA21:AM21"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="K20:S20"/>
-    <mergeCell ref="T20:Z20"/>
-    <mergeCell ref="AA20:AM20"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K19:S19"/>
-    <mergeCell ref="T19:Z19"/>
-    <mergeCell ref="AA19:AM19"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K18:S18"/>
-    <mergeCell ref="T18:Z18"/>
-    <mergeCell ref="AA18:AM18"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="K17:S17"/>
-    <mergeCell ref="T17:Z17"/>
-    <mergeCell ref="AA17:AM17"/>
-    <mergeCell ref="D14:AJ15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:S16"/>
-    <mergeCell ref="T16:Z16"/>
-    <mergeCell ref="AA16:AM16"/>
     <mergeCell ref="AB8:AE9"/>
     <mergeCell ref="AF8:AI9"/>
     <mergeCell ref="AJ8:AM9"/>
@@ -3006,6 +2909,103 @@
     <mergeCell ref="AF7:AI7"/>
     <mergeCell ref="AJ7:AM7"/>
     <mergeCell ref="C6:Y10"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="K17:S17"/>
+    <mergeCell ref="T17:Z17"/>
+    <mergeCell ref="AA17:AM17"/>
+    <mergeCell ref="D14:AJ15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:S16"/>
+    <mergeCell ref="T16:Z16"/>
+    <mergeCell ref="AA16:AM16"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="K19:S19"/>
+    <mergeCell ref="T19:Z19"/>
+    <mergeCell ref="AA19:AM19"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K18:S18"/>
+    <mergeCell ref="T18:Z18"/>
+    <mergeCell ref="AA18:AM18"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:S21"/>
+    <mergeCell ref="T21:Z21"/>
+    <mergeCell ref="AA21:AM21"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="K20:S20"/>
+    <mergeCell ref="T20:Z20"/>
+    <mergeCell ref="AA20:AM20"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:S23"/>
+    <mergeCell ref="T23:Z23"/>
+    <mergeCell ref="AA23:AM23"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:S22"/>
+    <mergeCell ref="T22:Z22"/>
+    <mergeCell ref="AA22:AM22"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="K25:S25"/>
+    <mergeCell ref="T25:Z25"/>
+    <mergeCell ref="AA25:AM25"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="K24:S24"/>
+    <mergeCell ref="T24:Z24"/>
+    <mergeCell ref="AA24:AM24"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="K27:S27"/>
+    <mergeCell ref="T27:Z27"/>
+    <mergeCell ref="AA27:AM27"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="K26:S26"/>
+    <mergeCell ref="T26:Z26"/>
+    <mergeCell ref="AA26:AM26"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="K29:S29"/>
+    <mergeCell ref="T29:Z29"/>
+    <mergeCell ref="AA29:AM29"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="K28:S28"/>
+    <mergeCell ref="T28:Z28"/>
+    <mergeCell ref="AA28:AM28"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="K31:S31"/>
+    <mergeCell ref="T31:Z31"/>
+    <mergeCell ref="AA31:AM31"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="K30:S30"/>
+    <mergeCell ref="T30:Z30"/>
+    <mergeCell ref="AA30:AM30"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23599999999999999" right="0.27500000000000002" top="0.51100000000000001" bottom="0.433" header="0.51100000000000001" footer="0.51100000000000001"/>

</xml_diff>